<commit_message>
Setup extra credit assignment
</commit_message>
<xml_diff>
--- a/softwareExecutionModeling/softwareexecutionmodel.xlsx
+++ b/softwareExecutionModeling/softwareexecutionmodel.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/rdavis2_stevens_edu/Documents/junior_year/ssw345-modeling_and_simulation/HW/softwareExecutionModeling/"/>
@@ -10,14 +10,14 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="72" documentId="8_{7433BD0D-002C-4A3A-B0C8-F436AE7493CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CF6B1C-6974-7244-AD0F-1D997DCC4709}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="27900" windowHeight="17500" activeTab="2" xr2:uid="{E6B6092C-0BC8-462B-A167-39153943AD0A}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="27900" windowHeight="17500" firstSheet="2" activeTab="2" xr2:uid="{E6B6092C-0BC8-462B-A167-39153943AD0A}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="1" r:id="rId1"/>
     <sheet name="5.2" sheetId="2" r:id="rId2"/>
     <sheet name="5.3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,15 +43,66 @@
     <t>P0</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>processing step</t>
+  </si>
+  <si>
+    <t>1x CPU (Kinst)</t>
+  </si>
+  <si>
+    <t>1x Disk (I/O)</t>
+  </si>
+  <si>
+    <t>1x Net (Msg)</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
     <t>openPage()</t>
   </si>
   <si>
+    <t>db</t>
+  </si>
+  <si>
     <t>getCriteria()</t>
   </si>
   <si>
+    <t>msg</t>
+  </si>
+  <si>
     <t>search()</t>
   </si>
   <si>
+    <t>execution time</t>
+  </si>
+  <si>
     <t>closePage()</t>
   </si>
   <si>
@@ -61,21 +112,18 @@
     <t>getItem()</t>
   </si>
   <si>
-    <t>processing step</t>
-  </si>
-  <si>
-    <t>1x CPU (Kinst)</t>
-  </si>
-  <si>
-    <t>1x Disk (I/O)</t>
-  </si>
-  <si>
-    <t>1x Net (Msg)</t>
-  </si>
-  <si>
     <t>TOTALS</t>
   </si>
   <si>
+    <t xml:space="preserve">Best demand time: </t>
+  </si>
+  <si>
+    <t>Worst Demand Time</t>
+  </si>
+  <si>
+    <t>Average demand time</t>
+  </si>
+  <si>
     <t>Overhead Matrix</t>
   </si>
   <si>
@@ -85,21 +133,21 @@
     <t>device</t>
   </si>
   <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Disk</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
     <t>service unit</t>
   </si>
   <si>
-    <t>CPU</t>
-  </si>
-  <si>
-    <t>Disk</t>
-  </si>
-  <si>
-    <t>Network</t>
-  </si>
-  <si>
     <t>Kinstructions</t>
   </si>
   <si>
@@ -127,52 +175,28 @@
     <t>service time</t>
   </si>
   <si>
-    <t>work</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>msg</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>execution time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best demand time: </t>
-  </si>
-  <si>
-    <t>Worst Demand Time</t>
-  </si>
-  <si>
-    <t>Average demand time</t>
-  </si>
-  <si>
-    <t>P13</t>
+    <t>initialize</t>
+  </si>
+  <si>
+    <t>case block</t>
+  </si>
+  <si>
+    <t>updateMirrorNY</t>
+  </si>
+  <si>
+    <t>UpdateMirrorLA</t>
+  </si>
+  <si>
+    <t>QueryMirrorNY</t>
+  </si>
+  <si>
+    <t>queryMirrorLA</t>
+  </si>
+  <si>
+    <t>writeMirrorNY</t>
+  </si>
+  <si>
+    <t>writeMirrorLA</t>
   </si>
   <si>
     <t>hardware</t>
@@ -182,30 +206,6 @@
   </si>
   <si>
     <t>Visits</t>
-  </si>
-  <si>
-    <t>initialize</t>
-  </si>
-  <si>
-    <t>case block</t>
-  </si>
-  <si>
-    <t>updateMirrorNY</t>
-  </si>
-  <si>
-    <t>UpdateMirrorLA</t>
-  </si>
-  <si>
-    <t>QueryMirrorNY</t>
-  </si>
-  <si>
-    <t>queryMirrorLA</t>
-  </si>
-  <si>
-    <t>writeMirrorNY</t>
-  </si>
-  <si>
-    <t>writeMirrorLA</t>
   </si>
   <si>
     <t>keywordSearch()</t>
@@ -239,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,10 +302,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -631,17 +627,17 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,48 +645,48 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>4</v>
@@ -720,9 +716,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -734,7 +730,7 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -764,9 +760,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>200</v>
@@ -778,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -808,9 +804,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -822,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <f>($B$23*$B$16*B9)+(C9*C16*C23)+(D9*D16*D23)</f>
@@ -865,9 +861,9 @@
         <v>20.382999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -879,9 +875,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -893,9 +889,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>220</v>
@@ -907,9 +903,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <f>SUM(B3:B8)</f>
@@ -924,60 +920,60 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="F10" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2">
         <f>MIN(SUM(G5,H5,G5,(SUM(I5,J5,G5, K5, L5)*4)), (SUM(G5,H5,G5,(SUM(I5,G5,G5)*4))), (SUM(G5,H5,G5,(SUM(I5,H5,G5)*4))), (SUM(G5,H5,G5,(SUM(I5,P5,G5)*4))))</f>
         <v>21.963999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="F11" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G11" s="2">
         <f>MAX(SUM(G5,H5,G5,(SUM(I5,J5,G5, K5, L5)*4)), (SUM(G5,H5,G5,(SUM(I5,G5,G5)*4))), (SUM(G5,H5,G5,(SUM(I5,H5,G5)*4))), (SUM(G5,H5,G5,(SUM(I5,P5,G5)*4))))</f>
         <v>101.524</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="F12" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G12" s="3">
         <f>SUM(G5,H5,G5,((I5+G5+J5*0.1+K5+L5+G5*0.2+0.3*H5+0.4*P5))*4)</f>
         <v>86.953999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -989,28 +985,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>400</v>
@@ -1022,9 +1018,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>1500</v>
@@ -1036,9 +1032,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -1050,14 +1046,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B23">
         <v>1E-4</v>
@@ -1082,48 +1078,48 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1150,16 +1146,16 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="L2" s="2">
         <f>MIN((2*SUM(B5,C5,D5)),(2*SUM(B5,C5,E5)),(2*SUM(B5,C5,F5)),(2*SUM(B5,C5,G5)),(2*SUM(B5,C5,H5)),(SUM(B5,C5,I5)))</f>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1186,16 +1182,16 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="L3" s="2">
         <f>MAX((2*SUM(B5,C5,D5)),(2*SUM(B5,C5,E5)),(2*SUM(B5,C5)),(2*SUM(B5,C5)),(2*SUM(B5,C5,H5)),(SUM(B5,C5,I5)))</f>
         <v>2.4250000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1222,16 +1218,16 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2">
         <f>2*(B5+C5+0.5*0.7*D5+0.3*E5+0.1*H5+0.1*I5)</f>
         <v>1.94225</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <f>($C$19*$C$12*(B2*$C$15+B3*$C$16+B4*$C$17))+($D$19*D12*(B2*$D$15+B3*$D$16+B4*$D$17))+($E$19*$E$12*(B2*$E$15+B3*$E$16+B4*$E$17))</f>
@@ -1266,31 +1262,31 @@
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1305,31 +1301,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -1344,9 +1340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>400</v>
@@ -1361,9 +1357,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>25</v>
@@ -1378,14 +1374,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>1E-4</v>
@@ -1413,21 +1409,21 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>56</v>
@@ -1439,7 +1435,7 @@
         <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
         <v>59</v>
@@ -1448,9 +1444,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>30</v>
@@ -1474,7 +1470,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1500,9 +1496,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1526,9 +1522,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <f>B2*$B$7*$B$8+B3*$C$7*$C$8+B4*$D$7*$D$8</f>
@@ -1559,20 +1555,20 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1584,9 +1580,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>1E-3</v>
@@ -1598,7 +1594,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="C12" t="s">
         <v>62</v>
       </c>
@@ -1607,7 +1603,7 @@
         <v>42.620000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="C13" t="s">
         <v>63</v>
       </c>
@@ -1616,7 +1612,7 @@
         <v>2.6200000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" t="s">
         <v>64</v>
       </c>

</xml_diff>